<commit_message>
Wird nicht mehr verwendet
</commit_message>
<xml_diff>
--- a/personData.xlsx
+++ b/personData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -23,196 +23,202 @@
     <t>SALARY</t>
   </si>
   <si>
+    <t>36.0</t>
+  </si>
+  <si>
+    <t>84.0</t>
+  </si>
+  <si>
+    <t>22.0</t>
+  </si>
+  <si>
+    <t>44.0</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>61.0</t>
+  </si>
+  <si>
+    <t>57.0</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>78.0</t>
+  </si>
+  <si>
+    <t>37.0</t>
+  </si>
+  <si>
+    <t>80.0</t>
+  </si>
+  <si>
+    <t>81.0</t>
+  </si>
+  <si>
+    <t>24.0</t>
+  </si>
+  <si>
+    <t>67.0</t>
+  </si>
+  <si>
+    <t>71.0</t>
+  </si>
+  <si>
+    <t>42.0</t>
+  </si>
+  <si>
+    <t>32.0</t>
+  </si>
+  <si>
+    <t>76.0</t>
+  </si>
+  <si>
+    <t>52.0</t>
+  </si>
+  <si>
+    <t>40.0</t>
+  </si>
+  <si>
+    <t>48.0</t>
+  </si>
+  <si>
+    <t>29.0</t>
+  </si>
+  <si>
+    <t>49.0</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>55.0</t>
+  </si>
+  <si>
+    <t>63.0</t>
+  </si>
+  <si>
+    <t>39.0</t>
+  </si>
+  <si>
+    <t>88.0</t>
+  </si>
+  <si>
+    <t>64.0</t>
+  </si>
+  <si>
+    <t>25.0</t>
+  </si>
+  <si>
     <t>26.0</t>
   </si>
   <si>
-    <t>42.0</t>
+    <t>41.0</t>
+  </si>
+  <si>
+    <t>79.0</t>
+  </si>
+  <si>
+    <t>43.0</t>
+  </si>
+  <si>
+    <t>59.0</t>
+  </si>
+  <si>
+    <t>51.0</t>
+  </si>
+  <si>
+    <t>77.0</t>
+  </si>
+  <si>
+    <t>72.0</t>
+  </si>
+  <si>
+    <t>47.0</t>
+  </si>
+  <si>
+    <t>58.0</t>
+  </si>
+  <si>
+    <t>45.0</t>
+  </si>
+  <si>
+    <t>46.0</t>
   </si>
   <si>
     <t>34.0</t>
   </si>
   <si>
-    <t>69.0</t>
-  </si>
-  <si>
-    <t>24.0</t>
+    <t>74.0</t>
+  </si>
+  <si>
+    <t>35.0</t>
+  </si>
+  <si>
+    <t>87.0</t>
+  </si>
+  <si>
+    <t>89.0</t>
+  </si>
+  <si>
+    <t>38.0</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>62.0</t>
+  </si>
+  <si>
+    <t>33.0</t>
+  </si>
+  <si>
+    <t>31.0</t>
+  </si>
+  <si>
+    <t>73.0</t>
+  </si>
+  <si>
+    <t>23.0</t>
+  </si>
+  <si>
+    <t>56.0</t>
   </si>
   <si>
     <t>68.0</t>
   </si>
   <si>
-    <t>40.0</t>
-  </si>
-  <si>
-    <t>76.0</t>
-  </si>
-  <si>
-    <t>31.0</t>
-  </si>
-  <si>
-    <t>55.0</t>
-  </si>
-  <si>
-    <t>36.0</t>
-  </si>
-  <si>
-    <t>54.0</t>
-  </si>
-  <si>
-    <t>25.0</t>
-  </si>
-  <si>
-    <t>44.0</t>
-  </si>
-  <si>
-    <t>86.0</t>
+    <t>27.0</t>
+  </si>
+  <si>
+    <t>66.0</t>
+  </si>
+  <si>
+    <t>28.0</t>
+  </si>
+  <si>
+    <t>82.0</t>
+  </si>
+  <si>
+    <t>70.0</t>
+  </si>
+  <si>
+    <t>60.0</t>
+  </si>
+  <si>
+    <t>53.0</t>
+  </si>
+  <si>
+    <t>85.0</t>
+  </si>
+  <si>
+    <t>75.0</t>
   </si>
   <si>
     <t>90.0</t>
-  </si>
-  <si>
-    <t>47.0</t>
-  </si>
-  <si>
-    <t>59.0</t>
-  </si>
-  <si>
-    <t>39.0</t>
-  </si>
-  <si>
-    <t>87.0</t>
-  </si>
-  <si>
-    <t>46.0</t>
-  </si>
-  <si>
-    <t>35.0</t>
-  </si>
-  <si>
-    <t>62.0</t>
-  </si>
-  <si>
-    <t>57.0</t>
-  </si>
-  <si>
-    <t>38.0</t>
-  </si>
-  <si>
-    <t>74.0</t>
-  </si>
-  <si>
-    <t>65.0</t>
-  </si>
-  <si>
-    <t>27.0</t>
-  </si>
-  <si>
-    <t>81.0</t>
-  </si>
-  <si>
-    <t>43.0</t>
-  </si>
-  <si>
-    <t>53.0</t>
-  </si>
-  <si>
-    <t>33.0</t>
-  </si>
-  <si>
-    <t>41.0</t>
-  </si>
-  <si>
-    <t>49.0</t>
-  </si>
-  <si>
-    <t>84.0</t>
-  </si>
-  <si>
-    <t>63.0</t>
-  </si>
-  <si>
-    <t>22.0</t>
-  </si>
-  <si>
-    <t>89.0</t>
-  </si>
-  <si>
-    <t>23.0</t>
-  </si>
-  <si>
-    <t>48.0</t>
-  </si>
-  <si>
-    <t>67.0</t>
-  </si>
-  <si>
-    <t>30.0</t>
-  </si>
-  <si>
-    <t>85.0</t>
-  </si>
-  <si>
-    <t>56.0</t>
-  </si>
-  <si>
-    <t>20.0</t>
-  </si>
-  <si>
-    <t>79.0</t>
-  </si>
-  <si>
-    <t>37.0</t>
-  </si>
-  <si>
-    <t>61.0</t>
-  </si>
-  <si>
-    <t>50.0</t>
-  </si>
-  <si>
-    <t>75.0</t>
-  </si>
-  <si>
-    <t>82.0</t>
-  </si>
-  <si>
-    <t>51.0</t>
-  </si>
-  <si>
-    <t>32.0</t>
-  </si>
-  <si>
-    <t>72.0</t>
-  </si>
-  <si>
-    <t>28.0</t>
-  </si>
-  <si>
-    <t>45.0</t>
-  </si>
-  <si>
-    <t>58.0</t>
-  </si>
-  <si>
-    <t>71.0</t>
-  </si>
-  <si>
-    <t>64.0</t>
-  </si>
-  <si>
-    <t>52.0</t>
-  </si>
-  <si>
-    <t>21.0</t>
-  </si>
-  <si>
-    <t>66.0</t>
-  </si>
-  <si>
-    <t>83.0</t>
-  </si>
-  <si>
-    <t>80.0</t>
   </si>
 </sst>
 </file>
@@ -312,10 +318,10 @@
         <v>11.0</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -323,10 +329,10 @@
         <v>12.0</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -334,10 +340,10 @@
         <v>13.0</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -345,7 +351,7 @@
         <v>14.0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -356,10 +362,10 @@
         <v>15.0</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
@@ -367,10 +373,10 @@
         <v>16.0</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -378,10 +384,10 @@
         <v>17.0</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -389,10 +395,10 @@
         <v>18.0</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -400,10 +406,10 @@
         <v>1.0</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
@@ -411,10 +417,10 @@
         <v>19.0</v>
       </c>
       <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -422,10 +428,10 @@
         <v>20.0</v>
       </c>
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="16">
@@ -433,10 +439,10 @@
         <v>21.0</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
@@ -444,10 +450,10 @@
         <v>22.0</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18">
@@ -455,10 +461,10 @@
         <v>23.0</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
@@ -466,7 +472,7 @@
         <v>24.0</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -477,10 +483,10 @@
         <v>25.0</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21">
@@ -488,10 +494,10 @@
         <v>26.0</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22">
@@ -499,10 +505,10 @@
         <v>27.0</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
@@ -510,10 +516,10 @@
         <v>28.0</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
@@ -524,7 +530,7 @@
         <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25">
@@ -532,10 +538,10 @@
         <v>29.0</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26">
@@ -543,10 +549,10 @@
         <v>30.0</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27">
@@ -554,10 +560,10 @@
         <v>31.0</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28">
@@ -565,10 +571,10 @@
         <v>32.0</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29">
@@ -576,10 +582,10 @@
         <v>33.0</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30">
@@ -587,10 +593,10 @@
         <v>34.0</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31">
@@ -598,10 +604,10 @@
         <v>35.0</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32">
@@ -609,10 +615,10 @@
         <v>36.0</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33">
@@ -620,10 +626,10 @@
         <v>37.0</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34">
@@ -631,10 +637,10 @@
         <v>38.0</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35">
@@ -645,7 +651,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36">
@@ -653,10 +659,10 @@
         <v>39.0</v>
       </c>
       <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
         <v>44</v>
-      </c>
-      <c r="C36" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="37">
@@ -664,10 +670,10 @@
         <v>40.0</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38">
@@ -675,10 +681,10 @@
         <v>41.0</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39">
@@ -686,10 +692,10 @@
         <v>42.0</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40">
@@ -697,10 +703,10 @@
         <v>43.0</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41">
@@ -708,10 +714,10 @@
         <v>44.0</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42">
@@ -719,10 +725,10 @@
         <v>45.0</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43">
@@ -730,10 +736,10 @@
         <v>46.0</v>
       </c>
       <c r="B43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" t="s">
         <v>42</v>
-      </c>
-      <c r="C43" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="44">
@@ -741,10 +747,10 @@
         <v>47.0</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45">
@@ -752,10 +758,10 @@
         <v>48.0</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46">
@@ -763,10 +769,10 @@
         <v>4.0</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47">
@@ -774,10 +780,10 @@
         <v>49.0</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48">
@@ -785,10 +791,10 @@
         <v>50.0</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49">
@@ -796,10 +802,10 @@
         <v>51.0</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
@@ -807,10 +813,10 @@
         <v>52.0</v>
       </c>
       <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" t="s">
         <v>55</v>
-      </c>
-      <c r="C50" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="51">
@@ -818,10 +824,10 @@
         <v>53.0</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C51" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52">
@@ -829,10 +835,10 @@
         <v>54.0</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53">
@@ -840,10 +846,10 @@
         <v>55.0</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54">
@@ -851,10 +857,10 @@
         <v>56.0</v>
       </c>
       <c r="B54" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55">
@@ -862,10 +868,10 @@
         <v>57.0</v>
       </c>
       <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" t="s">
         <v>57</v>
-      </c>
-      <c r="C55" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="56">
@@ -873,10 +879,10 @@
         <v>58.0</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="57">
@@ -884,10 +890,10 @@
         <v>5.0</v>
       </c>
       <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" t="s">
         <v>58</v>
-      </c>
-      <c r="C57" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="58">
@@ -895,10 +901,10 @@
         <v>59.0</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59">
@@ -906,10 +912,10 @@
         <v>60.0</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60">
@@ -917,10 +923,10 @@
         <v>61.0</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61">
@@ -928,10 +934,10 @@
         <v>62.0</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62">
@@ -939,10 +945,10 @@
         <v>63.0</v>
       </c>
       <c r="B62" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63">
@@ -950,10 +956,10 @@
         <v>64.0</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64">
@@ -961,10 +967,10 @@
         <v>65.0</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65">
@@ -972,10 +978,10 @@
         <v>66.0</v>
       </c>
       <c r="B65" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66">
@@ -983,10 +989,10 @@
         <v>67.0</v>
       </c>
       <c r="B66" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67">
@@ -994,10 +1000,10 @@
         <v>68.0</v>
       </c>
       <c r="B67" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C67" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68">
@@ -1005,10 +1011,10 @@
         <v>6.0</v>
       </c>
       <c r="B68" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C68" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69">
@@ -1016,10 +1022,10 @@
         <v>69.0</v>
       </c>
       <c r="B69" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70">
@@ -1027,10 +1033,10 @@
         <v>70.0</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C70" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71">
@@ -1038,10 +1044,10 @@
         <v>71.0</v>
       </c>
       <c r="B71" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C71" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72">
@@ -1049,10 +1055,10 @@
         <v>72.0</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C72" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73">
@@ -1060,10 +1066,10 @@
         <v>73.0</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C73" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74">
@@ -1071,10 +1077,10 @@
         <v>74.0</v>
       </c>
       <c r="B74" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75">
@@ -1082,10 +1088,10 @@
         <v>75.0</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C75" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76">
@@ -1093,10 +1099,10 @@
         <v>76.0</v>
       </c>
       <c r="B76" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C76" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="77">
@@ -1104,10 +1110,10 @@
         <v>77.0</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78">
@@ -1115,10 +1121,10 @@
         <v>78.0</v>
       </c>
       <c r="B78" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C78" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79">
@@ -1126,10 +1132,10 @@
         <v>7.0</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80">
@@ -1137,10 +1143,10 @@
         <v>79.0</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C80" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81">
@@ -1148,10 +1154,10 @@
         <v>80.0</v>
       </c>
       <c r="B81" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C81" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82">
@@ -1159,10 +1165,10 @@
         <v>81.0</v>
       </c>
       <c r="B82" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C82" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83">
@@ -1170,10 +1176,10 @@
         <v>82.0</v>
       </c>
       <c r="B83" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84">
@@ -1181,10 +1187,10 @@
         <v>83.0</v>
       </c>
       <c r="B84" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85">
@@ -1192,10 +1198,10 @@
         <v>84.0</v>
       </c>
       <c r="B85" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C85" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="86">
@@ -1203,10 +1209,10 @@
         <v>85.0</v>
       </c>
       <c r="B86" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C86" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87">
@@ -1214,10 +1220,10 @@
         <v>86.0</v>
       </c>
       <c r="B87" t="s">
+        <v>54</v>
+      </c>
+      <c r="C87" t="s">
         <v>27</v>
-      </c>
-      <c r="C87" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="88">
@@ -1225,10 +1231,10 @@
         <v>87.0</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C88" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89">
@@ -1236,10 +1242,10 @@
         <v>88.0</v>
       </c>
       <c r="B89" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C89" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90">
@@ -1247,10 +1253,10 @@
         <v>8.0</v>
       </c>
       <c r="B90" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91">
@@ -1258,10 +1264,10 @@
         <v>89.0</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C91" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>